<commit_message>
Required data for interpolation
</commit_message>
<xml_diff>
--- a/data/interpolation_parameters.xlsx
+++ b/data/interpolation_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\ghnfarid\Projects\meteo-interp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B63259E-9D49-4CE0-BDDA-D553AB239832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DAADA0-6E6B-4DDC-9F44-876D428E6DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -148,7 +148,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,7 +463,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,13 +503,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
@@ -518,10 +518,10 @@
         <v>35</v>
       </c>
       <c r="F2" s="2">
-        <v>38353</v>
+        <v>43831</v>
       </c>
       <c r="G2" s="2">
-        <v>38399</v>
+        <v>43834</v>
       </c>
     </row>
   </sheetData>

</xml_diff>